<commit_message>
fixed script and schema definition in Excel
</commit_message>
<xml_diff>
--- a/app/Vendor/db/schema/attributes.xlsx
+++ b/app/Vendor/db/schema/attributes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
   <si>
     <t>ColumnID</t>
   </si>
@@ -88,15 +88,9 @@
     <t>auto_increment</t>
   </si>
   <si>
-    <t>ringStatus</t>
-  </si>
-  <si>
     <t>承認結果</t>
   </si>
   <si>
-    <t>tinyint(1)</t>
-  </si>
-  <si>
     <t>Code management in the 'name' master</t>
   </si>
   <si>
@@ -112,10 +106,10 @@
     <t>更新ID</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t>Disable</t>
+  </si>
+  <si>
+    <t>ringiStatus</t>
   </si>
 </sst>
 </file>
@@ -944,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,7 +974,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1100,33 +1094,33 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
         <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
@@ -1146,10 +1140,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -1164,20 +1158,6 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>